<commit_message>
Fix rutas absolutas para compatibilidad en Render
</commit_message>
<xml_diff>
--- a/BaseFinalDni.xlsx
+++ b/BaseFinalDni.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E408"/>
+  <dimension ref="A1:E479"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11449,6 +11449,1923 @@
         </is>
       </c>
     </row>
+    <row r="409">
+      <c r="A409" t="inlineStr">
+        <is>
+          <t>No encontrado</t>
+        </is>
+      </c>
+      <c r="B409" t="inlineStr">
+        <is>
+          <t>Dante Dora B De</t>
+        </is>
+      </c>
+      <c r="C409" t="inlineStr">
+        <is>
+          <t>(11) 4214 - 6531</t>
+        </is>
+      </c>
+      <c r="D409" t="inlineStr">
+        <is>
+          <t>Quintana 630 PB CASA</t>
+        </is>
+      </c>
+      <c r="E409" t="inlineStr">
+        <is>
+          <t>Adrogué - Buenos Aires (CP:1846)</t>
+        </is>
+      </c>
+    </row>
+    <row r="410">
+      <c r="A410" t="inlineStr">
+        <is>
+          <t>20-04372373-2</t>
+        </is>
+      </c>
+      <c r="B410" t="inlineStr">
+        <is>
+          <t>Dante Humberto R</t>
+        </is>
+      </c>
+      <c r="C410" t="inlineStr">
+        <is>
+          <t>(11) 4294 - 4681</t>
+        </is>
+      </c>
+      <c r="D410" t="inlineStr">
+        <is>
+          <t>Av T Espora 1165 PB</t>
+        </is>
+      </c>
+      <c r="E410" t="inlineStr">
+        <is>
+          <t>Adrogué - Buenos Aires (CP:1846)</t>
+        </is>
+      </c>
+    </row>
+    <row r="411">
+      <c r="A411" t="inlineStr">
+        <is>
+          <t>No encontrado</t>
+        </is>
+      </c>
+      <c r="B411" t="inlineStr">
+        <is>
+          <t>Lanfranchini Dante</t>
+        </is>
+      </c>
+      <c r="C411" t="inlineStr">
+        <is>
+          <t>(11) 4294 - 1253</t>
+        </is>
+      </c>
+      <c r="D411" t="inlineStr">
+        <is>
+          <t>Int GonzÃ¡lez 1694 PB FTE</t>
+        </is>
+      </c>
+      <c r="E411" t="inlineStr">
+        <is>
+          <t>Adrogué - Buenos Aires (CP:1846)</t>
+        </is>
+      </c>
+    </row>
+    <row r="412">
+      <c r="A412" t="inlineStr">
+        <is>
+          <t>20-04377366-7</t>
+        </is>
+      </c>
+      <c r="B412" t="inlineStr">
+        <is>
+          <t>Mariani Dante</t>
+        </is>
+      </c>
+      <c r="C412" t="inlineStr">
+        <is>
+          <t>(11) 4294 - 7533</t>
+        </is>
+      </c>
+      <c r="D412" t="inlineStr">
+        <is>
+          <t>De Kay 793 PB</t>
+        </is>
+      </c>
+      <c r="E412" t="inlineStr">
+        <is>
+          <t>Adrogué - Buenos Aires (CP:1846)</t>
+        </is>
+      </c>
+    </row>
+    <row r="413">
+      <c r="A413" t="inlineStr">
+        <is>
+          <t>20-14331415-5</t>
+        </is>
+      </c>
+      <c r="B413" t="inlineStr">
+        <is>
+          <t>Reynoso Dante M</t>
+        </is>
+      </c>
+      <c r="C413" t="inlineStr">
+        <is>
+          <t>(11) 4293 - 1306</t>
+        </is>
+      </c>
+      <c r="D413" t="inlineStr">
+        <is>
+          <t>A Erezcano 1570</t>
+        </is>
+      </c>
+      <c r="E413" t="inlineStr">
+        <is>
+          <t>Adrogué - Buenos Aires (CP:1846)</t>
+        </is>
+      </c>
+    </row>
+    <row r="414">
+      <c r="A414" t="inlineStr">
+        <is>
+          <t>20-06603032-7</t>
+        </is>
+      </c>
+      <c r="B414" t="inlineStr">
+        <is>
+          <t>Rodriguez Dante D</t>
+        </is>
+      </c>
+      <c r="C414" t="inlineStr">
+        <is>
+          <t>(11) 4669 - 2688</t>
+        </is>
+      </c>
+      <c r="D414" t="inlineStr">
+        <is>
+          <t>Pje L Fresias 570</t>
+        </is>
+      </c>
+      <c r="E414" t="inlineStr">
+        <is>
+          <t>Malvinas Argentinas Adrogué - Buenos Aires (CP:1851)</t>
+        </is>
+      </c>
+    </row>
+    <row r="415">
+      <c r="A415" t="inlineStr">
+        <is>
+          <t>20-16558915-8</t>
+        </is>
+      </c>
+      <c r="B415" t="inlineStr">
+        <is>
+          <t>Tegli Dante O</t>
+        </is>
+      </c>
+      <c r="C415" t="inlineStr">
+        <is>
+          <t>(11) 4293 - 3677</t>
+        </is>
+      </c>
+      <c r="D415" t="inlineStr">
+        <is>
+          <t>Serrano 197 PB CASA</t>
+        </is>
+      </c>
+      <c r="E415" t="inlineStr">
+        <is>
+          <t>Malvinas Argentinas Adrogué - Buenos Aires (CP:1851)</t>
+        </is>
+      </c>
+    </row>
+    <row r="416">
+      <c r="A416" t="inlineStr">
+        <is>
+          <t>20-07372324-9</t>
+        </is>
+      </c>
+      <c r="B416" t="inlineStr">
+        <is>
+          <t>Gomez Dionisio D</t>
+        </is>
+      </c>
+      <c r="C416" t="inlineStr">
+        <is>
+          <t>(11) 4293 - 0589</t>
+        </is>
+      </c>
+      <c r="D416" t="inlineStr">
+        <is>
+          <t>Retiro 1146</t>
+        </is>
+      </c>
+      <c r="E416" t="inlineStr">
+        <is>
+          <t>Malvinas Argentinas Adrogué - Buenos Aires (CP:1851)</t>
+        </is>
+      </c>
+    </row>
+    <row r="417">
+      <c r="A417" t="inlineStr">
+        <is>
+          <t>20-03085886-8</t>
+        </is>
+      </c>
+      <c r="B417" t="inlineStr">
+        <is>
+          <t>Arduino Domingo A</t>
+        </is>
+      </c>
+      <c r="C417" t="inlineStr">
+        <is>
+          <t>(3401) 48 - 0276</t>
+        </is>
+      </c>
+      <c r="D417" t="inlineStr">
+        <is>
+          <t>Mazzini 421</t>
+        </is>
+      </c>
+      <c r="E417" t="inlineStr">
+        <is>
+          <t>Carlos Pellegrini - Santa Fe (CP:2453)</t>
+        </is>
+      </c>
+    </row>
+    <row r="418">
+      <c r="A418" t="inlineStr">
+        <is>
+          <t>20-04638701-6</t>
+        </is>
+      </c>
+      <c r="B418" t="inlineStr">
+        <is>
+          <t>Barreto Domingo R</t>
+        </is>
+      </c>
+      <c r="C418" t="inlineStr">
+        <is>
+          <t>(11) 4293 - 6311</t>
+        </is>
+      </c>
+      <c r="D418" t="inlineStr">
+        <is>
+          <t>B Q MartÃ­n 698</t>
+        </is>
+      </c>
+      <c r="E418" t="inlineStr">
+        <is>
+          <t>Malvinas Argentinas Adrogué - Buenos Aires (CP:1851)</t>
+        </is>
+      </c>
+    </row>
+    <row r="419">
+      <c r="A419" t="inlineStr">
+        <is>
+          <t>20-05900959-2</t>
+        </is>
+      </c>
+      <c r="B419" t="inlineStr">
+        <is>
+          <t>Carnuccio Domingo N</t>
+        </is>
+      </c>
+      <c r="C419" t="inlineStr">
+        <is>
+          <t>(11) 4293 - 9101</t>
+        </is>
+      </c>
+      <c r="D419" t="inlineStr">
+        <is>
+          <t>Canale 1795 PB</t>
+        </is>
+      </c>
+      <c r="E419" t="inlineStr">
+        <is>
+          <t>Adrogué - Buenos Aires (CP:1846)</t>
+        </is>
+      </c>
+    </row>
+    <row r="420">
+      <c r="A420" t="inlineStr">
+        <is>
+          <t>20-07763624-3</t>
+        </is>
+      </c>
+      <c r="B420" t="inlineStr">
+        <is>
+          <t>Carrique Domingo M</t>
+        </is>
+      </c>
+      <c r="C420" t="inlineStr">
+        <is>
+          <t>(11) 4293 - 3057</t>
+        </is>
+      </c>
+      <c r="D420" t="inlineStr">
+        <is>
+          <t>De Kay 1273 PB CASA</t>
+        </is>
+      </c>
+      <c r="E420" t="inlineStr">
+        <is>
+          <t>Adrogué - Buenos Aires (CP:1846)</t>
+        </is>
+      </c>
+    </row>
+    <row r="421">
+      <c r="A421" t="inlineStr">
+        <is>
+          <t>20-05294507-1</t>
+        </is>
+      </c>
+      <c r="B421" t="inlineStr">
+        <is>
+          <t>Castillo Domingo B</t>
+        </is>
+      </c>
+      <c r="C421" t="inlineStr">
+        <is>
+          <t>(11) 4214 - 0510</t>
+        </is>
+      </c>
+      <c r="D421" t="inlineStr">
+        <is>
+          <t>J Soto Acebal 53 PA</t>
+        </is>
+      </c>
+      <c r="E421" t="inlineStr">
+        <is>
+          <t>Malvinas Argentinas Adrogué - Buenos Aires (CP:1851)</t>
+        </is>
+      </c>
+    </row>
+    <row r="422">
+      <c r="A422" t="inlineStr">
+        <is>
+          <t>20-06420074-8</t>
+        </is>
+      </c>
+      <c r="B422" t="inlineStr">
+        <is>
+          <t>Cravero Domingo</t>
+        </is>
+      </c>
+      <c r="C422" t="inlineStr">
+        <is>
+          <t>(3401) 48 - 0096</t>
+        </is>
+      </c>
+      <c r="D422" t="inlineStr">
+        <is>
+          <t>Avellaneda 566</t>
+        </is>
+      </c>
+      <c r="E422" t="inlineStr">
+        <is>
+          <t>Carlos Pellegrini - Santa Fe (CP:2453)</t>
+        </is>
+      </c>
+    </row>
+    <row r="423">
+      <c r="A423" t="inlineStr">
+        <is>
+          <t>20-60735412-0</t>
+        </is>
+      </c>
+      <c r="B423" t="inlineStr">
+        <is>
+          <t>D'andrea Domingo</t>
+        </is>
+      </c>
+      <c r="C423" t="inlineStr">
+        <is>
+          <t>(11) 4293 - 7692</t>
+        </is>
+      </c>
+      <c r="D423" t="inlineStr">
+        <is>
+          <t>E AdroguÃ© 1045 1 B</t>
+        </is>
+      </c>
+      <c r="E423" t="inlineStr">
+        <is>
+          <t>Adrogué - Buenos Aires (CP:1846)</t>
+        </is>
+      </c>
+    </row>
+    <row r="424">
+      <c r="A424" t="inlineStr">
+        <is>
+          <t>20-07793346-9</t>
+        </is>
+      </c>
+      <c r="B424" t="inlineStr">
+        <is>
+          <t>Di Buccio Domingo O</t>
+        </is>
+      </c>
+      <c r="C424" t="inlineStr">
+        <is>
+          <t>(11) 4294 - 4061</t>
+        </is>
+      </c>
+      <c r="D424" t="inlineStr">
+        <is>
+          <t>F SeguÃ­ 843 PB</t>
+        </is>
+      </c>
+      <c r="E424" t="inlineStr">
+        <is>
+          <t>Adrogué - Buenos Aires (CP:1846)</t>
+        </is>
+      </c>
+    </row>
+    <row r="425">
+      <c r="A425" t="inlineStr">
+        <is>
+          <t>20-15206243-6</t>
+        </is>
+      </c>
+      <c r="B425" t="inlineStr">
+        <is>
+          <t>Domingo Stella M</t>
+        </is>
+      </c>
+      <c r="C425" t="inlineStr">
+        <is>
+          <t>(11) 4294 - 8464</t>
+        </is>
+      </c>
+      <c r="D425" t="inlineStr">
+        <is>
+          <t>E Pettoruti 19 PB</t>
+        </is>
+      </c>
+      <c r="E425" t="inlineStr">
+        <is>
+          <t>Malvinas Argentinas Adrogué - Buenos Aires (CP:1851)</t>
+        </is>
+      </c>
+    </row>
+    <row r="426">
+      <c r="A426" t="inlineStr">
+        <is>
+          <t>20-15206243-6</t>
+        </is>
+      </c>
+      <c r="B426" t="inlineStr">
+        <is>
+          <t>Domingo Stella M</t>
+        </is>
+      </c>
+      <c r="C426" t="inlineStr">
+        <is>
+          <t>(11) 4294 - 0987</t>
+        </is>
+      </c>
+      <c r="D426" t="inlineStr">
+        <is>
+          <t>E Pettoruti 19 PB</t>
+        </is>
+      </c>
+      <c r="E426" t="inlineStr">
+        <is>
+          <t>Malvinas Argentinas Adrogué - Buenos Aires (CP:1851)</t>
+        </is>
+      </c>
+    </row>
+    <row r="427">
+      <c r="A427" t="inlineStr">
+        <is>
+          <t>20-93507603-0</t>
+        </is>
+      </c>
+      <c r="B427" t="inlineStr">
+        <is>
+          <t>Fino Domingo</t>
+        </is>
+      </c>
+      <c r="C427" t="inlineStr">
+        <is>
+          <t>(11) 4294 - 2040</t>
+        </is>
+      </c>
+      <c r="D427" t="inlineStr">
+        <is>
+          <t>C RamÃ­rez 1233 PB</t>
+        </is>
+      </c>
+      <c r="E427" t="inlineStr">
+        <is>
+          <t>Adrogué - Buenos Aires (CP:1846)</t>
+        </is>
+      </c>
+    </row>
+    <row r="428">
+      <c r="A428" t="inlineStr">
+        <is>
+          <t>20-05337266-0</t>
+        </is>
+      </c>
+      <c r="B428" t="inlineStr">
+        <is>
+          <t>Goni Domingo F</t>
+        </is>
+      </c>
+      <c r="C428" t="inlineStr">
+        <is>
+          <t>(11) 6066 - 8065</t>
+        </is>
+      </c>
+      <c r="D428" t="inlineStr">
+        <is>
+          <t>Cap Moyano 1633</t>
+        </is>
+      </c>
+      <c r="E428" t="inlineStr">
+        <is>
+          <t>Malvinas Argentinas Adrogué - Buenos Aires (CP:1851)</t>
+        </is>
+      </c>
+    </row>
+    <row r="429">
+      <c r="A429" t="inlineStr">
+        <is>
+          <t>No encontrado</t>
+        </is>
+      </c>
+      <c r="B429" t="inlineStr">
+        <is>
+          <t>Goã‘i Domingo</t>
+        </is>
+      </c>
+      <c r="C429" t="inlineStr">
+        <is>
+          <t>(11) 4293 - 7695</t>
+        </is>
+      </c>
+      <c r="D429" t="inlineStr">
+        <is>
+          <t>Derqui 343 PB</t>
+        </is>
+      </c>
+      <c r="E429" t="inlineStr">
+        <is>
+          <t>Malvinas Argentinas Adrogué - Buenos Aires (CP:1851)</t>
+        </is>
+      </c>
+    </row>
+    <row r="430">
+      <c r="A430" t="inlineStr">
+        <is>
+          <t>33-55834117-9</t>
+        </is>
+      </c>
+      <c r="B430" t="inlineStr">
+        <is>
+          <t>Guzzetta Domingo</t>
+        </is>
+      </c>
+      <c r="C430" t="inlineStr">
+        <is>
+          <t>(11) 4294 - 3556</t>
+        </is>
+      </c>
+      <c r="D430" t="inlineStr">
+        <is>
+          <t>H Bouchard 1430 PB 14</t>
+        </is>
+      </c>
+      <c r="E430" t="inlineStr">
+        <is>
+          <t>Adrogué - Buenos Aires (CP:1846)</t>
+        </is>
+      </c>
+    </row>
+    <row r="431">
+      <c r="A431" t="inlineStr">
+        <is>
+          <t>23-05136492-9</t>
+        </is>
+      </c>
+      <c r="B431" t="inlineStr">
+        <is>
+          <t>Laera Domingo</t>
+        </is>
+      </c>
+      <c r="C431" t="inlineStr">
+        <is>
+          <t>(11) 4294 - 8562</t>
+        </is>
+      </c>
+      <c r="D431" t="inlineStr">
+        <is>
+          <t>T Taylor 1441 PB</t>
+        </is>
+      </c>
+      <c r="E431" t="inlineStr">
+        <is>
+          <t>Adrogué - Buenos Aires (CP:1846)</t>
+        </is>
+      </c>
+    </row>
+    <row r="432">
+      <c r="A432" t="inlineStr">
+        <is>
+          <t>No encontrado</t>
+        </is>
+      </c>
+      <c r="B432" t="inlineStr">
+        <is>
+          <t>Rossi Vergara Edmundo</t>
+        </is>
+      </c>
+      <c r="C432" t="inlineStr">
+        <is>
+          <t>(11) 4294 - 8577</t>
+        </is>
+      </c>
+      <c r="D432" t="inlineStr">
+        <is>
+          <t>J D De SolÃ­s 1615 PB</t>
+        </is>
+      </c>
+      <c r="E432" t="inlineStr">
+        <is>
+          <t>Adrogué - Buenos Aires (CP:1846)</t>
+        </is>
+      </c>
+    </row>
+    <row r="433">
+      <c r="A433" t="inlineStr">
+        <is>
+          <t>No encontrado</t>
+        </is>
+      </c>
+      <c r="B433" t="inlineStr">
+        <is>
+          <t>Aguino Elena L De</t>
+        </is>
+      </c>
+      <c r="C433" t="inlineStr">
+        <is>
+          <t>(11) 4294 - 9976</t>
+        </is>
+      </c>
+      <c r="D433" t="inlineStr">
+        <is>
+          <t>E Policastro 375</t>
+        </is>
+      </c>
+      <c r="E433" t="inlineStr">
+        <is>
+          <t>Malvinas Argentinas Adrogué - Buenos Aires (CP:1851)</t>
+        </is>
+      </c>
+    </row>
+    <row r="434">
+      <c r="A434" t="inlineStr">
+        <is>
+          <t>27-00250184-3</t>
+        </is>
+      </c>
+      <c r="B434" t="inlineStr">
+        <is>
+          <t>Airoldi Elena R</t>
+        </is>
+      </c>
+      <c r="C434" t="inlineStr">
+        <is>
+          <t>(11) 4294 - 4657</t>
+        </is>
+      </c>
+      <c r="D434" t="inlineStr">
+        <is>
+          <t>H Bouchard 1516 PB</t>
+        </is>
+      </c>
+      <c r="E434" t="inlineStr">
+        <is>
+          <t>Adrogué - Buenos Aires (CP:1846)</t>
+        </is>
+      </c>
+    </row>
+    <row r="435">
+      <c r="A435" t="inlineStr">
+        <is>
+          <t>27-02022410-5</t>
+        </is>
+      </c>
+      <c r="B435" t="inlineStr">
+        <is>
+          <t>Alessi Elena M</t>
+        </is>
+      </c>
+      <c r="C435" t="inlineStr">
+        <is>
+          <t>(11) 4294 - 0540</t>
+        </is>
+      </c>
+      <c r="D435" t="inlineStr">
+        <is>
+          <t>Mitre 1656</t>
+        </is>
+      </c>
+      <c r="E435" t="inlineStr">
+        <is>
+          <t>Adrogué - Buenos Aires (CP:1846)</t>
+        </is>
+      </c>
+    </row>
+    <row r="436">
+      <c r="A436" t="inlineStr">
+        <is>
+          <t>27-02471766-1</t>
+        </is>
+      </c>
+      <c r="B436" t="inlineStr">
+        <is>
+          <t>Asenjo Elena H</t>
+        </is>
+      </c>
+      <c r="C436" t="inlineStr">
+        <is>
+          <t>(11) 4294 - 4939</t>
+        </is>
+      </c>
+      <c r="D436" t="inlineStr">
+        <is>
+          <t>Av T Espora 969</t>
+        </is>
+      </c>
+      <c r="E436" t="inlineStr">
+        <is>
+          <t>Adrogué - Buenos Aires (CP:1846)</t>
+        </is>
+      </c>
+    </row>
+    <row r="437">
+      <c r="A437" t="inlineStr">
+        <is>
+          <t>No encontrado</t>
+        </is>
+      </c>
+      <c r="B437" t="inlineStr">
+        <is>
+          <t>Barretta Elena R De</t>
+        </is>
+      </c>
+      <c r="C437" t="inlineStr">
+        <is>
+          <t>(11) 4214 - 7648</t>
+        </is>
+      </c>
+      <c r="D437" t="inlineStr">
+        <is>
+          <t>Av T Espora 351 PB</t>
+        </is>
+      </c>
+      <c r="E437" t="inlineStr">
+        <is>
+          <t>Adrogué - Buenos Aires (CP:1846)</t>
+        </is>
+      </c>
+    </row>
+    <row r="438">
+      <c r="A438" t="inlineStr">
+        <is>
+          <t>No encontrado</t>
+        </is>
+      </c>
+      <c r="B438" t="inlineStr">
+        <is>
+          <t>Capilla Elena L P De</t>
+        </is>
+      </c>
+      <c r="C438" t="inlineStr">
+        <is>
+          <t>(11) 4299 - 1698</t>
+        </is>
+      </c>
+      <c r="D438" t="inlineStr">
+        <is>
+          <t>Dr L Pasteur 555 PB</t>
+        </is>
+      </c>
+      <c r="E438" t="inlineStr">
+        <is>
+          <t>Malvinas Argentinas Adrogué - Buenos Aires (CP:1846)</t>
+        </is>
+      </c>
+    </row>
+    <row r="439">
+      <c r="A439" t="inlineStr">
+        <is>
+          <t>27-01744729-2</t>
+        </is>
+      </c>
+      <c r="B439" t="inlineStr">
+        <is>
+          <t>Cartavio Elena D</t>
+        </is>
+      </c>
+      <c r="C439" t="inlineStr">
+        <is>
+          <t>(11) 4293 - 1921</t>
+        </is>
+      </c>
+      <c r="D439" t="inlineStr">
+        <is>
+          <t>J De La PeÃ±a 60 PB FTE</t>
+        </is>
+      </c>
+      <c r="E439" t="inlineStr">
+        <is>
+          <t>Adrogué - Buenos Aires (CP:1846)</t>
+        </is>
+      </c>
+    </row>
+    <row r="440">
+      <c r="A440" t="inlineStr">
+        <is>
+          <t>23-01354739-4</t>
+        </is>
+      </c>
+      <c r="B440" t="inlineStr">
+        <is>
+          <t>Castell Elena M</t>
+        </is>
+      </c>
+      <c r="C440" t="inlineStr">
+        <is>
+          <t>(11) 4214 - 0337</t>
+        </is>
+      </c>
+      <c r="D440" t="inlineStr">
+        <is>
+          <t>J E Hunter 29 2 4</t>
+        </is>
+      </c>
+      <c r="E440" t="inlineStr">
+        <is>
+          <t>Adrogué - Buenos Aires (CP:1846)</t>
+        </is>
+      </c>
+    </row>
+    <row r="441">
+      <c r="A441" t="inlineStr">
+        <is>
+          <t>27-00211175-1</t>
+        </is>
+      </c>
+      <c r="B441" t="inlineStr">
+        <is>
+          <t>Chirino Elena T</t>
+        </is>
+      </c>
+      <c r="C441" t="inlineStr">
+        <is>
+          <t>(11) 4284 - 2311</t>
+        </is>
+      </c>
+      <c r="D441" t="inlineStr">
+        <is>
+          <t>Serrano 3458</t>
+        </is>
+      </c>
+      <c r="E441" t="inlineStr">
+        <is>
+          <t>Malvinas Argentinas Adrogué - Buenos Aires (CP:1851)</t>
+        </is>
+      </c>
+    </row>
+    <row r="442">
+      <c r="A442" t="inlineStr">
+        <is>
+          <t>27-13597975-4</t>
+        </is>
+      </c>
+      <c r="B442" t="inlineStr">
+        <is>
+          <t>Constantinidis Elena</t>
+        </is>
+      </c>
+      <c r="C442" t="inlineStr">
+        <is>
+          <t>(11) 4293 - 2733</t>
+        </is>
+      </c>
+      <c r="D442" t="inlineStr">
+        <is>
+          <t>Soler 311</t>
+        </is>
+      </c>
+      <c r="E442" t="inlineStr">
+        <is>
+          <t>Malvinas Argentinas Adrogué - Buenos Aires (CP:1851)</t>
+        </is>
+      </c>
+    </row>
+    <row r="443">
+      <c r="A443" t="inlineStr">
+        <is>
+          <t>27-02151401-8</t>
+        </is>
+      </c>
+      <c r="B443" t="inlineStr">
+        <is>
+          <t>Corbetta Elena</t>
+        </is>
+      </c>
+      <c r="C443" t="inlineStr">
+        <is>
+          <t>(11) 4214 - 0564</t>
+        </is>
+      </c>
+      <c r="D443" t="inlineStr">
+        <is>
+          <t>A De Angonelli 1555 PB</t>
+        </is>
+      </c>
+      <c r="E443" t="inlineStr">
+        <is>
+          <t>Adrogué - Buenos Aires (CP:1846)</t>
+        </is>
+      </c>
+    </row>
+    <row r="444">
+      <c r="A444" t="inlineStr">
+        <is>
+          <t>20-41556586-1</t>
+        </is>
+      </c>
+      <c r="B444" t="inlineStr">
+        <is>
+          <t>Elena Lucas E</t>
+        </is>
+      </c>
+      <c r="C444" t="inlineStr">
+        <is>
+          <t>(11) 6073 - 7252</t>
+        </is>
+      </c>
+      <c r="D444" t="inlineStr">
+        <is>
+          <t>A Illia 1290</t>
+        </is>
+      </c>
+      <c r="E444" t="inlineStr">
+        <is>
+          <t>Adrogué - Buenos Aires (CP:1846)</t>
+        </is>
+      </c>
+    </row>
+    <row r="445">
+      <c r="A445" t="inlineStr">
+        <is>
+          <t>20-05844177-6</t>
+        </is>
+      </c>
+      <c r="B445" t="inlineStr">
+        <is>
+          <t>Elena Manuel</t>
+        </is>
+      </c>
+      <c r="C445" t="inlineStr">
+        <is>
+          <t>(11) 4293 - 3694</t>
+        </is>
+      </c>
+      <c r="D445" t="inlineStr">
+        <is>
+          <t>Av T Espora 1755 1 A</t>
+        </is>
+      </c>
+      <c r="E445" t="inlineStr">
+        <is>
+          <t>Adrogué - Buenos Aires (CP:1846)</t>
+        </is>
+      </c>
+    </row>
+    <row r="446">
+      <c r="A446" t="inlineStr">
+        <is>
+          <t>23-05334310-4</t>
+        </is>
+      </c>
+      <c r="B446" t="inlineStr">
+        <is>
+          <t>Elena Maria</t>
+        </is>
+      </c>
+      <c r="C446" t="inlineStr">
+        <is>
+          <t>(11) 4293 - 5164</t>
+        </is>
+      </c>
+      <c r="D446" t="inlineStr">
+        <is>
+          <t>M DemarÃ­a 1250 PB FTE</t>
+        </is>
+      </c>
+      <c r="E446" t="inlineStr">
+        <is>
+          <t>Adrogué - Buenos Aires (CP:1846)</t>
+        </is>
+      </c>
+    </row>
+    <row r="447">
+      <c r="A447" t="inlineStr">
+        <is>
+          <t>27-05353440-1</t>
+        </is>
+      </c>
+      <c r="B447" t="inlineStr">
+        <is>
+          <t>Enrique Elena</t>
+        </is>
+      </c>
+      <c r="C447" t="inlineStr">
+        <is>
+          <t>(11) 4297 - 9231</t>
+        </is>
+      </c>
+      <c r="D447" t="inlineStr">
+        <is>
+          <t>E Policastro 2112</t>
+        </is>
+      </c>
+      <c r="E447" t="inlineStr">
+        <is>
+          <t>Malvinas Argentinas Adrogué - Buenos Aires (CP:1851)</t>
+        </is>
+      </c>
+    </row>
+    <row r="448">
+      <c r="A448" t="inlineStr">
+        <is>
+          <t>20-28585555-2</t>
+        </is>
+      </c>
+      <c r="B448" t="inlineStr">
+        <is>
+          <t>Buceta Emanuel G</t>
+        </is>
+      </c>
+      <c r="C448" t="inlineStr">
+        <is>
+          <t>(11) 4293 - 5487</t>
+        </is>
+      </c>
+      <c r="D448" t="inlineStr">
+        <is>
+          <t>Av H Yrigoyen 13448</t>
+        </is>
+      </c>
+      <c r="E448" t="inlineStr">
+        <is>
+          <t>Adrogué - Buenos Aires (CP:1846)</t>
+        </is>
+      </c>
+    </row>
+    <row r="449">
+      <c r="A449" t="inlineStr">
+        <is>
+          <t>20-28585555-2</t>
+        </is>
+      </c>
+      <c r="B449" t="inlineStr">
+        <is>
+          <t>Buceta Emanuel G</t>
+        </is>
+      </c>
+      <c r="C449" t="inlineStr">
+        <is>
+          <t>(11) 6061 - 0954</t>
+        </is>
+      </c>
+      <c r="D449" t="inlineStr">
+        <is>
+          <t>Av H Yrigoyen 13448</t>
+        </is>
+      </c>
+      <c r="E449" t="inlineStr">
+        <is>
+          <t>Adrogué - Buenos Aires (CP:1846)</t>
+        </is>
+      </c>
+    </row>
+    <row r="450">
+      <c r="A450" t="inlineStr">
+        <is>
+          <t>20-32086962-6</t>
+        </is>
+      </c>
+      <c r="B450" t="inlineStr">
+        <is>
+          <t>Friscione Bruno Emanuel</t>
+        </is>
+      </c>
+      <c r="C450" t="inlineStr">
+        <is>
+          <t>(3401) 48 - 1016</t>
+        </is>
+      </c>
+      <c r="D450" t="inlineStr">
+        <is>
+          <t>Gral Rawson 509</t>
+        </is>
+      </c>
+      <c r="E450" t="inlineStr">
+        <is>
+          <t>Carlos Pellegrini - Santa Fe (CP:2453)</t>
+        </is>
+      </c>
+    </row>
+    <row r="451">
+      <c r="A451" t="inlineStr">
+        <is>
+          <t>20-30356123-5</t>
+        </is>
+      </c>
+      <c r="B451" t="inlineStr">
+        <is>
+          <t>Saavedra Emanuel</t>
+        </is>
+      </c>
+      <c r="C451" t="inlineStr">
+        <is>
+          <t>(11) 4263 - 0886</t>
+        </is>
+      </c>
+      <c r="D451" t="inlineStr">
+        <is>
+          <t>Pino 4089 PB 2</t>
+        </is>
+      </c>
+      <c r="E451" t="inlineStr">
+        <is>
+          <t>Malvinas Argentinas Adrogué - Buenos Aires (CP:1851)</t>
+        </is>
+      </c>
+    </row>
+    <row r="452">
+      <c r="A452" t="inlineStr">
+        <is>
+          <t>20-27374391-0</t>
+        </is>
+      </c>
+      <c r="B452" t="inlineStr">
+        <is>
+          <t>Vera Emanuel</t>
+        </is>
+      </c>
+      <c r="C452" t="inlineStr">
+        <is>
+          <t>(11) 4880 - 7063</t>
+        </is>
+      </c>
+      <c r="D452" t="inlineStr">
+        <is>
+          <t>Ob J Colombres 1513 PB FTE</t>
+        </is>
+      </c>
+      <c r="E452" t="inlineStr">
+        <is>
+          <t>Adrogué - Buenos Aires (CP:1846)</t>
+        </is>
+      </c>
+    </row>
+    <row r="453">
+      <c r="A453" t="inlineStr">
+        <is>
+          <t>20-31790862-9</t>
+        </is>
+      </c>
+      <c r="B453" t="inlineStr">
+        <is>
+          <t>Villa Emanuel A</t>
+        </is>
+      </c>
+      <c r="C453" t="inlineStr">
+        <is>
+          <t>(3854) 49 - 0988</t>
+        </is>
+      </c>
+      <c r="D453" t="inlineStr">
+        <is>
+          <t>Calle PÃºblica S/N</t>
+        </is>
+      </c>
+      <c r="E453" t="inlineStr">
+        <is>
+          <t>Choya - Santiago del Estero (CP:4233)</t>
+        </is>
+      </c>
+    </row>
+    <row r="454">
+      <c r="A454" t="inlineStr">
+        <is>
+          <t>No encontrado</t>
+        </is>
+      </c>
+      <c r="B454" t="inlineStr">
+        <is>
+          <t>Azurabarrena Emilio</t>
+        </is>
+      </c>
+      <c r="C454" t="inlineStr">
+        <is>
+          <t>(11) 4294 - 2345</t>
+        </is>
+      </c>
+      <c r="D454" t="inlineStr">
+        <is>
+          <t>Quintana 564 PB</t>
+        </is>
+      </c>
+      <c r="E454" t="inlineStr">
+        <is>
+          <t>Adrogué - Buenos Aires (CP:1846)</t>
+        </is>
+      </c>
+    </row>
+    <row r="455">
+      <c r="A455" t="inlineStr">
+        <is>
+          <t>20-05655570-7</t>
+        </is>
+      </c>
+      <c r="B455" t="inlineStr">
+        <is>
+          <t>Durand Emilio L</t>
+        </is>
+      </c>
+      <c r="C455" t="inlineStr">
+        <is>
+          <t>(11) 4297 - 7769</t>
+        </is>
+      </c>
+      <c r="D455" t="inlineStr">
+        <is>
+          <t>Int E Carmona 420</t>
+        </is>
+      </c>
+      <c r="E455" t="inlineStr">
+        <is>
+          <t>Malvinas Argentinas Adrogué - Buenos Aires (CP:1851)</t>
+        </is>
+      </c>
+    </row>
+    <row r="456">
+      <c r="A456" t="inlineStr">
+        <is>
+          <t>20-04280651-0</t>
+        </is>
+      </c>
+      <c r="B456" t="inlineStr">
+        <is>
+          <t>Fuertes Emilio</t>
+        </is>
+      </c>
+      <c r="C456" t="inlineStr">
+        <is>
+          <t>(11) 4294 - 6643</t>
+        </is>
+      </c>
+      <c r="D456" t="inlineStr">
+        <is>
+          <t>Ej Argentino 651 1 8</t>
+        </is>
+      </c>
+      <c r="E456" t="inlineStr">
+        <is>
+          <t>Adrogué - Buenos Aires (CP:1846)</t>
+        </is>
+      </c>
+    </row>
+    <row r="457">
+      <c r="A457" t="inlineStr">
+        <is>
+          <t>20-00067363-4</t>
+        </is>
+      </c>
+      <c r="B457" t="inlineStr">
+        <is>
+          <t>Gianolli Emilio A</t>
+        </is>
+      </c>
+      <c r="C457" t="inlineStr">
+        <is>
+          <t>(11) 4294 - 4920</t>
+        </is>
+      </c>
+      <c r="D457" t="inlineStr">
+        <is>
+          <t>PavÃ³n 120 PB</t>
+        </is>
+      </c>
+      <c r="E457" t="inlineStr">
+        <is>
+          <t>Adrogué - Buenos Aires (CP:1846)</t>
+        </is>
+      </c>
+    </row>
+    <row r="458">
+      <c r="A458" t="inlineStr">
+        <is>
+          <t>20-04965579-8</t>
+        </is>
+      </c>
+      <c r="B458" t="inlineStr">
+        <is>
+          <t>Gutierrez Emilio</t>
+        </is>
+      </c>
+      <c r="C458" t="inlineStr">
+        <is>
+          <t>(11) 4214 - 3216</t>
+        </is>
+      </c>
+      <c r="D458" t="inlineStr">
+        <is>
+          <t>Comb De Juncal 1081</t>
+        </is>
+      </c>
+      <c r="E458" t="inlineStr">
+        <is>
+          <t>Adrogué - Buenos Aires (CP:1846)</t>
+        </is>
+      </c>
+    </row>
+    <row r="459">
+      <c r="A459" t="inlineStr">
+        <is>
+          <t>20-08380345-3</t>
+        </is>
+      </c>
+      <c r="B459" t="inlineStr">
+        <is>
+          <t>Jerez Emilio J</t>
+        </is>
+      </c>
+      <c r="C459" t="inlineStr">
+        <is>
+          <t>(11) 4297 - 7647</t>
+        </is>
+      </c>
+      <c r="D459" t="inlineStr">
+        <is>
+          <t>Bs Aires 70 PB CASA</t>
+        </is>
+      </c>
+      <c r="E459" t="inlineStr">
+        <is>
+          <t>Malvinas Argentinas Adrogué - Buenos Aires (CP:1851)</t>
+        </is>
+      </c>
+    </row>
+    <row r="460">
+      <c r="A460" t="inlineStr">
+        <is>
+          <t>20-01914200-1</t>
+        </is>
+      </c>
+      <c r="B460" t="inlineStr">
+        <is>
+          <t>Karles Emilio</t>
+        </is>
+      </c>
+      <c r="C460" t="inlineStr">
+        <is>
+          <t>(11) 4294 - 1680</t>
+        </is>
+      </c>
+      <c r="D460" t="inlineStr">
+        <is>
+          <t>T Taylor 1141</t>
+        </is>
+      </c>
+      <c r="E460" t="inlineStr">
+        <is>
+          <t>Adrogué - Buenos Aires (CP:1846)</t>
+        </is>
+      </c>
+    </row>
+    <row r="461">
+      <c r="A461" t="inlineStr">
+        <is>
+          <t>20-14802298-5</t>
+        </is>
+      </c>
+      <c r="B461" t="inlineStr">
+        <is>
+          <t>Klubus Emilio E</t>
+        </is>
+      </c>
+      <c r="C461" t="inlineStr">
+        <is>
+          <t>(11) 4294 - 6088</t>
+        </is>
+      </c>
+      <c r="D461" t="inlineStr">
+        <is>
+          <t>E Obligado 1245</t>
+        </is>
+      </c>
+      <c r="E461" t="inlineStr">
+        <is>
+          <t>Adrogué - Buenos Aires (CP:1846)</t>
+        </is>
+      </c>
+    </row>
+    <row r="462">
+      <c r="A462" t="inlineStr">
+        <is>
+          <t>20-07456054-8</t>
+        </is>
+      </c>
+      <c r="B462" t="inlineStr">
+        <is>
+          <t>Kotas Emilio M</t>
+        </is>
+      </c>
+      <c r="C462" t="inlineStr">
+        <is>
+          <t>(11) 4297 - 8870</t>
+        </is>
+      </c>
+      <c r="D462" t="inlineStr">
+        <is>
+          <t>Retiro 2155 PB</t>
+        </is>
+      </c>
+      <c r="E462" t="inlineStr">
+        <is>
+          <t>Malvinas Argentinas Adrogué - Buenos Aires (CP:1851)</t>
+        </is>
+      </c>
+    </row>
+    <row r="463">
+      <c r="A463" t="inlineStr">
+        <is>
+          <t>20-00616760-9</t>
+        </is>
+      </c>
+      <c r="B463" t="inlineStr">
+        <is>
+          <t>Mattalia Emilio</t>
+        </is>
+      </c>
+      <c r="C463" t="inlineStr">
+        <is>
+          <t>(3401) 48 - 0439</t>
+        </is>
+      </c>
+      <c r="D463" t="inlineStr">
+        <is>
+          <t>M De Oca 542</t>
+        </is>
+      </c>
+      <c r="E463" t="inlineStr">
+        <is>
+          <t>Carlos Pellegrini - Santa Fe (CP:2453)</t>
+        </is>
+      </c>
+    </row>
+    <row r="464">
+      <c r="A464" t="inlineStr">
+        <is>
+          <t>23-07728276-9</t>
+        </is>
+      </c>
+      <c r="B464" t="inlineStr">
+        <is>
+          <t>Nazzari Emilio A</t>
+        </is>
+      </c>
+      <c r="C464" t="inlineStr">
+        <is>
+          <t>(11) 4294 - 1327</t>
+        </is>
+      </c>
+      <c r="D464" t="inlineStr">
+        <is>
+          <t>C RamÃ­rez 1802</t>
+        </is>
+      </c>
+      <c r="E464" t="inlineStr">
+        <is>
+          <t>Adrogué - Buenos Aires (CP:1846)</t>
+        </is>
+      </c>
+    </row>
+    <row r="465">
+      <c r="A465" t="inlineStr">
+        <is>
+          <t>20-11846972-1</t>
+        </is>
+      </c>
+      <c r="B465" t="inlineStr">
+        <is>
+          <t>Sabatino Emilio N</t>
+        </is>
+      </c>
+      <c r="C465" t="inlineStr">
+        <is>
+          <t>(11) 4293 - 2908</t>
+        </is>
+      </c>
+      <c r="D465" t="inlineStr">
+        <is>
+          <t>Int GonzÃ¡lez 330</t>
+        </is>
+      </c>
+      <c r="E465" t="inlineStr">
+        <is>
+          <t>Adrogué - Buenos Aires (CP:1846)</t>
+        </is>
+      </c>
+    </row>
+    <row r="466">
+      <c r="A466" t="inlineStr">
+        <is>
+          <t>20-04464608-1</t>
+        </is>
+      </c>
+      <c r="B466" t="inlineStr">
+        <is>
+          <t>Sanchez Sanchez Emilio</t>
+        </is>
+      </c>
+      <c r="C466" t="inlineStr">
+        <is>
+          <t>(11) 4294 - 1647</t>
+        </is>
+      </c>
+      <c r="D466" t="inlineStr">
+        <is>
+          <t>J A FrÃ­as 323 PB</t>
+        </is>
+      </c>
+      <c r="E466" t="inlineStr">
+        <is>
+          <t>Adrogué - Buenos Aires (CP:1846)</t>
+        </is>
+      </c>
+    </row>
+    <row r="467">
+      <c r="A467" t="inlineStr">
+        <is>
+          <t>20-04645260-8</t>
+        </is>
+      </c>
+      <c r="B467" t="inlineStr">
+        <is>
+          <t>Sempe Emilio A</t>
+        </is>
+      </c>
+      <c r="C467" t="inlineStr">
+        <is>
+          <t>(11) 4293 - 0152</t>
+        </is>
+      </c>
+      <c r="D467" t="inlineStr">
+        <is>
+          <t>M RodrÃ­guez 1153 PB</t>
+        </is>
+      </c>
+      <c r="E467" t="inlineStr">
+        <is>
+          <t>Adrogué - Buenos Aires (CP:1846)</t>
+        </is>
+      </c>
+    </row>
+    <row r="468">
+      <c r="A468" t="inlineStr">
+        <is>
+          <t>20-07754528-0</t>
+        </is>
+      </c>
+      <c r="B468" t="inlineStr">
+        <is>
+          <t>Torano Emilio</t>
+        </is>
+      </c>
+      <c r="C468" t="inlineStr">
+        <is>
+          <t>(11) 4294 - 0143</t>
+        </is>
+      </c>
+      <c r="D468" t="inlineStr">
+        <is>
+          <t>Amenedo 579 PB</t>
+        </is>
+      </c>
+      <c r="E468" t="inlineStr">
+        <is>
+          <t>Adrogué - Buenos Aires (CP:1846)</t>
+        </is>
+      </c>
+    </row>
+    <row r="469">
+      <c r="A469" t="inlineStr">
+        <is>
+          <t>No encontrado</t>
+        </is>
+      </c>
+      <c r="B469" t="inlineStr">
+        <is>
+          <t>Apphatie Esteban M</t>
+        </is>
+      </c>
+      <c r="C469" t="inlineStr">
+        <is>
+          <t>(11) 4294 - 4442</t>
+        </is>
+      </c>
+      <c r="D469" t="inlineStr">
+        <is>
+          <t>Av H Yrigoyen 13020 PB</t>
+        </is>
+      </c>
+      <c r="E469" t="inlineStr">
+        <is>
+          <t>Adrogué - Buenos Aires (CP:1846)</t>
+        </is>
+      </c>
+    </row>
+    <row r="470">
+      <c r="A470" t="inlineStr">
+        <is>
+          <t>20-05761888-5</t>
+        </is>
+      </c>
+      <c r="B470" t="inlineStr">
+        <is>
+          <t>Aquino Esteban</t>
+        </is>
+      </c>
+      <c r="C470" t="inlineStr">
+        <is>
+          <t>(3401) 48 - 0402</t>
+        </is>
+      </c>
+      <c r="D470" t="inlineStr">
+        <is>
+          <t>Gral Roca 1251</t>
+        </is>
+      </c>
+      <c r="E470" t="inlineStr">
+        <is>
+          <t>Carlos Pellegrini - Santa Fe (CP:2453)</t>
+        </is>
+      </c>
+    </row>
+    <row r="471">
+      <c r="A471" t="inlineStr">
+        <is>
+          <t>No encontrado</t>
+        </is>
+      </c>
+      <c r="B471" t="inlineStr">
+        <is>
+          <t>Asociacion Amigos Biblioteca Esteban</t>
+        </is>
+      </c>
+      <c r="C471" t="inlineStr">
+        <is>
+          <t>(11) 4214 - 4192</t>
+        </is>
+      </c>
+      <c r="D471" t="inlineStr">
+        <is>
+          <t>La Rosa 974</t>
+        </is>
+      </c>
+      <c r="E471" t="inlineStr">
+        <is>
+          <t>Adrogué - Buenos Aires (CP:1846)</t>
+        </is>
+      </c>
+    </row>
+    <row r="472">
+      <c r="A472" t="inlineStr">
+        <is>
+          <t>20-06395599-0</t>
+        </is>
+      </c>
+      <c r="B472" t="inlineStr">
+        <is>
+          <t>Bertolotti Esteban A</t>
+        </is>
+      </c>
+      <c r="C472" t="inlineStr">
+        <is>
+          <t>(3401) 48 - 0267</t>
+        </is>
+      </c>
+      <c r="D472" t="inlineStr">
+        <is>
+          <t>Alte Brown 953</t>
+        </is>
+      </c>
+      <c r="E472" t="inlineStr">
+        <is>
+          <t>Carlos Pellegrini - Santa Fe (CP:2453)</t>
+        </is>
+      </c>
+    </row>
+    <row r="473">
+      <c r="A473" t="inlineStr">
+        <is>
+          <t>20-10983909-5</t>
+        </is>
+      </c>
+      <c r="B473" t="inlineStr">
+        <is>
+          <t>Carreras Esteban G</t>
+        </is>
+      </c>
+      <c r="C473" t="inlineStr">
+        <is>
+          <t>(11) 4294 - 9463</t>
+        </is>
+      </c>
+      <c r="D473" t="inlineStr">
+        <is>
+          <t>C Pellegrini 996 PB</t>
+        </is>
+      </c>
+      <c r="E473" t="inlineStr">
+        <is>
+          <t>Adrogué - Buenos Aires (CP:1846)</t>
+        </is>
+      </c>
+    </row>
+    <row r="474">
+      <c r="A474" t="inlineStr">
+        <is>
+          <t>20-12813097-8</t>
+        </is>
+      </c>
+      <c r="B474" t="inlineStr">
+        <is>
+          <t>Corley Esteban</t>
+        </is>
+      </c>
+      <c r="C474" t="inlineStr">
+        <is>
+          <t>(11) 4294 - 6407</t>
+        </is>
+      </c>
+      <c r="D474" t="inlineStr">
+        <is>
+          <t>L Rosales 1156 PB</t>
+        </is>
+      </c>
+      <c r="E474" t="inlineStr">
+        <is>
+          <t>Adrogué - Buenos Aires (CP:1846)</t>
+        </is>
+      </c>
+    </row>
+    <row r="475">
+      <c r="A475" t="inlineStr">
+        <is>
+          <t>20-12813097-8</t>
+        </is>
+      </c>
+      <c r="B475" t="inlineStr">
+        <is>
+          <t>Corley Esteban G</t>
+        </is>
+      </c>
+      <c r="C475" t="inlineStr">
+        <is>
+          <t>(11) 4294 - 1239</t>
+        </is>
+      </c>
+      <c r="D475" t="inlineStr">
+        <is>
+          <t>L Rosales 1145</t>
+        </is>
+      </c>
+      <c r="E475" t="inlineStr">
+        <is>
+          <t>Adrogué - Buenos Aires (CP:1846)</t>
+        </is>
+      </c>
+    </row>
+    <row r="476">
+      <c r="A476" t="inlineStr">
+        <is>
+          <t>20-42621441-6</t>
+        </is>
+      </c>
+      <c r="B476" t="inlineStr">
+        <is>
+          <t>Desimone Esteban</t>
+        </is>
+      </c>
+      <c r="C476" t="inlineStr">
+        <is>
+          <t>(11) 4294 - 5831</t>
+        </is>
+      </c>
+      <c r="D476" t="inlineStr">
+        <is>
+          <t>Av T Espora 801 PB LOC</t>
+        </is>
+      </c>
+      <c r="E476" t="inlineStr">
+        <is>
+          <t>Adrogué - Buenos Aires (CP:1846)</t>
+        </is>
+      </c>
+    </row>
+    <row r="477">
+      <c r="A477" t="inlineStr">
+        <is>
+          <t>20-42621441-6</t>
+        </is>
+      </c>
+      <c r="B477" t="inlineStr">
+        <is>
+          <t>Desimone Esteban</t>
+        </is>
+      </c>
+      <c r="C477" t="inlineStr">
+        <is>
+          <t>(11) 4294 - 6220</t>
+        </is>
+      </c>
+      <c r="D477" t="inlineStr">
+        <is>
+          <t>Av T Espora 801 PB</t>
+        </is>
+      </c>
+      <c r="E477" t="inlineStr">
+        <is>
+          <t>Adrogué - Buenos Aires (CP:1846)</t>
+        </is>
+      </c>
+    </row>
+    <row r="478">
+      <c r="A478" t="inlineStr">
+        <is>
+          <t>20-42621441-6</t>
+        </is>
+      </c>
+      <c r="B478" t="inlineStr">
+        <is>
+          <t>Desimone Esteban</t>
+        </is>
+      </c>
+      <c r="C478" t="inlineStr">
+        <is>
+          <t>(11) 4294 - 6249</t>
+        </is>
+      </c>
+      <c r="D478" t="inlineStr">
+        <is>
+          <t>Av T Espora 801 PB LOC</t>
+        </is>
+      </c>
+      <c r="E478" t="inlineStr">
+        <is>
+          <t>Adrogué - Buenos Aires (CP:1846)</t>
+        </is>
+      </c>
+    </row>
+    <row r="479">
+      <c r="A479" t="inlineStr">
+        <is>
+          <t>20-04048632-2</t>
+        </is>
+      </c>
+      <c r="B479" t="inlineStr">
+        <is>
+          <t>Durand Esteban</t>
+        </is>
+      </c>
+      <c r="C479" t="inlineStr">
+        <is>
+          <t>(11) 4297 - 7642</t>
+        </is>
+      </c>
+      <c r="D479" t="inlineStr">
+        <is>
+          <t>Serrano 2011 PB</t>
+        </is>
+      </c>
+      <c r="E479" t="inlineStr">
+        <is>
+          <t>Malvinas Argentinas Adrogué - Buenos Aires (CP:1851)</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>